<commit_message>
[feature/ms-555] fix translate excel
</commit_message>
<xml_diff>
--- a/apps/core/fimport/static/fimport/template/import-hr-shift.xlsx
+++ b/apps/core/fimport/static/fimport/template/import-hr-shift.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCAdmin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8884CD-697D-473C-B83B-0A677FBAB5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A237FA48-6EA0-4E59-BA60-8813F60241B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A28B6FBF-5A4D-44A5-9537-9A8777902B4B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>Morning Shift</t>
   </si>
@@ -142,6 +142,15 @@
   </si>
   <si>
     <t>Ngày làm việc</t>
+  </si>
+  <si>
+    <t>Thời gian bắt đầu gia hạn giờ ra</t>
+  </si>
+  <si>
+    <t>Thời gian kết thúc gia hạn giờ ra</t>
+  </si>
+  <si>
+    <t>Ngưỡng trễ sớm giờ ra</t>
   </si>
 </sst>
 </file>
@@ -519,7 +528,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -591,13 +600,13 @@
         <v>32</v>
       </c>
       <c r="P1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="Q1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="R1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="S1" t="s">
         <v>33</v>

</xml_diff>